<commit_message>
substituindo valores do enunciado pelas variaveis
</commit_message>
<xml_diff>
--- a/P4/simulacao.xlsx
+++ b/P4/simulacao.xlsx
@@ -485,28 +485,28 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="C2" t="n">
+        <v>130</v>
+      </c>
+      <c r="D2" t="n">
         <v>80</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>75</v>
       </c>
-      <c r="E2" t="n">
-        <v>170</v>
-      </c>
       <c r="F2" t="n">
-        <v>515</v>
+        <v>743</v>
       </c>
       <c r="G2" t="n">
-        <v>421</v>
+        <v>560</v>
       </c>
       <c r="H2" t="n">
-        <v>6750</v>
+        <v>7200</v>
       </c>
       <c r="I2" t="n">
-        <v>-550</v>
+        <v>10875</v>
       </c>
     </row>
     <row r="3">
@@ -514,28 +514,28 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="C3" t="n">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="D3" t="n">
-        <v>150</v>
+        <v>75</v>
       </c>
       <c r="E3" t="n">
-        <v>110</v>
+        <v>75</v>
       </c>
       <c r="F3" t="n">
-        <v>500</v>
+        <v>443</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>255</v>
       </c>
       <c r="H3" t="n">
-        <v>9000</v>
+        <v>6750</v>
       </c>
       <c r="I3" t="n">
-        <v>15950</v>
+        <v>10875</v>
       </c>
     </row>
     <row r="4">
@@ -543,7 +543,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="C4" t="n">
         <v>130</v>
@@ -552,10 +552,10 @@
         <v>60</v>
       </c>
       <c r="E4" t="n">
-        <v>75</v>
+        <v>110</v>
       </c>
       <c r="F4" t="n">
-        <v>730</v>
+        <v>603</v>
       </c>
       <c r="G4" t="n">
         <v>400</v>
@@ -564,7 +564,7 @@
         <v>5400</v>
       </c>
       <c r="I4" t="n">
-        <v>10875</v>
+        <v>15950</v>
       </c>
     </row>
     <row r="5">
@@ -572,28 +572,28 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="C5" t="n">
-        <v>95</v>
+        <v>130</v>
       </c>
       <c r="D5" t="n">
         <v>80</v>
       </c>
       <c r="E5" t="n">
-        <v>170</v>
+        <v>110</v>
       </c>
       <c r="F5" t="n">
-        <v>730</v>
+        <v>723</v>
       </c>
       <c r="G5" t="n">
-        <v>515</v>
+        <v>410</v>
       </c>
       <c r="H5" t="n">
         <v>7200</v>
       </c>
       <c r="I5" t="n">
-        <v>3650</v>
+        <v>15950</v>
       </c>
     </row>
     <row r="6">
@@ -601,28 +601,28 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="C6" t="n">
-        <v>95</v>
+        <v>160</v>
       </c>
       <c r="D6" t="n">
-        <v>150</v>
+        <v>60</v>
       </c>
       <c r="E6" t="n">
         <v>130</v>
       </c>
       <c r="F6" t="n">
-        <v>670</v>
+        <v>343</v>
       </c>
       <c r="G6" t="n">
         <v>400</v>
       </c>
       <c r="H6" t="n">
-        <v>3000</v>
+        <v>5400</v>
       </c>
       <c r="I6" t="n">
-        <v>9050</v>
+        <v>18850</v>
       </c>
     </row>
     <row r="7">
@@ -630,10 +630,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>80</v>
+        <v>130</v>
       </c>
       <c r="C7" t="n">
-        <v>95</v>
+        <v>140</v>
       </c>
       <c r="D7" t="n">
         <v>150</v>
@@ -642,13 +642,13 @@
         <v>90</v>
       </c>
       <c r="F7" t="n">
-        <v>690</v>
+        <v>500</v>
       </c>
       <c r="G7" t="n">
         <v>400</v>
       </c>
       <c r="H7" t="n">
-        <v>3000</v>
+        <v>10500</v>
       </c>
       <c r="I7" t="n">
         <v>13050</v>
@@ -659,28 +659,28 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="C8" t="n">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="D8" t="n">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="E8" t="n">
-        <v>75</v>
+        <v>110</v>
       </c>
       <c r="F8" t="n">
-        <v>640</v>
+        <v>500</v>
       </c>
       <c r="G8" t="n">
         <v>400</v>
       </c>
       <c r="H8" t="n">
-        <v>7500</v>
+        <v>3000</v>
       </c>
       <c r="I8" t="n">
-        <v>10875</v>
+        <v>15950</v>
       </c>
     </row>
     <row r="9">
@@ -688,28 +688,28 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="C9" t="n">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="D9" t="n">
-        <v>80</v>
+        <v>150</v>
       </c>
       <c r="E9" t="n">
-        <v>75</v>
+        <v>110</v>
       </c>
       <c r="F9" t="n">
-        <v>330</v>
+        <v>500</v>
       </c>
       <c r="G9" t="n">
         <v>400</v>
       </c>
       <c r="H9" t="n">
-        <v>7200</v>
+        <v>4500</v>
       </c>
       <c r="I9" t="n">
-        <v>10875</v>
+        <v>7550</v>
       </c>
     </row>
     <row r="10">
@@ -717,28 +717,28 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="C10" t="n">
         <v>110</v>
       </c>
       <c r="D10" t="n">
-        <v>150</v>
+        <v>180</v>
       </c>
       <c r="E10" t="n">
-        <v>130</v>
+        <v>75</v>
       </c>
       <c r="F10" t="n">
         <v>500</v>
       </c>
       <c r="G10" t="n">
-        <v>495</v>
+        <v>400</v>
       </c>
       <c r="H10" t="n">
-        <v>4500</v>
+        <v>-300</v>
       </c>
       <c r="I10" t="n">
-        <v>13250</v>
+        <v>10875</v>
       </c>
     </row>
     <row r="11">
@@ -746,28 +746,28 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="C11" t="n">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="D11" t="n">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E11" t="n">
-        <v>90</v>
+        <v>170</v>
       </c>
       <c r="F11" t="n">
-        <v>660</v>
+        <v>510</v>
       </c>
       <c r="G11" t="n">
         <v>400</v>
       </c>
       <c r="H11" t="n">
-        <v>7200</v>
+        <v>6750</v>
       </c>
       <c r="I11" t="n">
-        <v>13050</v>
+        <v>3650</v>
       </c>
     </row>
     <row r="12">
@@ -781,22 +781,22 @@
         <v>110</v>
       </c>
       <c r="D12" t="n">
-        <v>180</v>
+        <v>60</v>
       </c>
       <c r="E12" t="n">
-        <v>75</v>
+        <v>130</v>
       </c>
       <c r="F12" t="n">
-        <v>650</v>
+        <v>630</v>
       </c>
       <c r="G12" t="n">
-        <v>450</v>
+        <v>400</v>
       </c>
       <c r="H12" t="n">
-        <v>-300</v>
+        <v>5400</v>
       </c>
       <c r="I12" t="n">
-        <v>10875</v>
+        <v>13250</v>
       </c>
     </row>
     <row r="13">
@@ -807,25 +807,25 @@
         <v>100</v>
       </c>
       <c r="C13" t="n">
-        <v>80</v>
+        <v>160</v>
       </c>
       <c r="D13" t="n">
-        <v>80</v>
+        <v>150</v>
       </c>
       <c r="E13" t="n">
-        <v>60</v>
+        <v>110</v>
       </c>
       <c r="F13" t="n">
-        <v>370</v>
+        <v>610</v>
       </c>
       <c r="G13" t="n">
-        <v>445</v>
+        <v>400</v>
       </c>
       <c r="H13" t="n">
-        <v>7200</v>
+        <v>6000</v>
       </c>
       <c r="I13" t="n">
-        <v>8700</v>
+        <v>15950</v>
       </c>
     </row>
     <row r="14">
@@ -833,28 +833,28 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="C14" t="n">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="D14" t="n">
         <v>180</v>
       </c>
       <c r="E14" t="n">
-        <v>130</v>
+        <v>75</v>
       </c>
       <c r="F14" t="n">
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="G14" t="n">
-        <v>585</v>
+        <v>400</v>
       </c>
       <c r="H14" t="n">
-        <v>4200</v>
+        <v>2700</v>
       </c>
       <c r="I14" t="n">
-        <v>13250</v>
+        <v>10875</v>
       </c>
     </row>
     <row r="15">
@@ -862,25 +862,25 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="C15" t="n">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="D15" t="n">
-        <v>180</v>
+        <v>60</v>
       </c>
       <c r="E15" t="n">
         <v>75</v>
       </c>
       <c r="F15" t="n">
-        <v>500</v>
+        <v>330</v>
       </c>
       <c r="G15" t="n">
-        <v>415</v>
+        <v>400</v>
       </c>
       <c r="H15" t="n">
-        <v>7200</v>
+        <v>5400</v>
       </c>
       <c r="I15" t="n">
         <v>10875</v>
@@ -891,28 +891,28 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="C16" t="n">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="D16" t="n">
-        <v>150</v>
+        <v>180</v>
       </c>
       <c r="E16" t="n">
-        <v>90</v>
+        <v>170</v>
       </c>
       <c r="F16" t="n">
-        <v>520</v>
+        <v>500</v>
       </c>
       <c r="G16" t="n">
-        <v>410</v>
+        <v>515</v>
       </c>
       <c r="H16" t="n">
-        <v>6000</v>
+        <v>-300</v>
       </c>
       <c r="I16" t="n">
-        <v>10250</v>
+        <v>3650</v>
       </c>
     </row>
     <row r="17">
@@ -920,28 +920,28 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="C17" t="n">
-        <v>110</v>
+        <v>160</v>
       </c>
       <c r="D17" t="n">
-        <v>150</v>
+        <v>80</v>
       </c>
       <c r="E17" t="n">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="F17" t="n">
-        <v>540</v>
+        <v>620</v>
       </c>
       <c r="G17" t="n">
         <v>400</v>
       </c>
       <c r="H17" t="n">
-        <v>9000</v>
+        <v>7200</v>
       </c>
       <c r="I17" t="n">
-        <v>13050</v>
+        <v>15950</v>
       </c>
     </row>
     <row r="18">
@@ -949,19 +949,19 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="C18" t="n">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="D18" t="n">
         <v>75</v>
       </c>
       <c r="E18" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="F18" t="n">
-        <v>770</v>
+        <v>790</v>
       </c>
       <c r="G18" t="n">
         <v>400</v>
@@ -970,7 +970,7 @@
         <v>6750</v>
       </c>
       <c r="I18" t="n">
-        <v>8700</v>
+        <v>13050</v>
       </c>
     </row>
     <row r="19">
@@ -978,28 +978,28 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
+        <v>100</v>
+      </c>
+      <c r="C19" t="n">
         <v>130</v>
       </c>
-      <c r="C19" t="n">
-        <v>80</v>
-      </c>
       <c r="D19" t="n">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="E19" t="n">
-        <v>75</v>
+        <v>110</v>
       </c>
       <c r="F19" t="n">
-        <v>470</v>
+        <v>450</v>
       </c>
       <c r="G19" t="n">
-        <v>545</v>
+        <v>455</v>
       </c>
       <c r="H19" t="n">
-        <v>6750</v>
+        <v>5400</v>
       </c>
       <c r="I19" t="n">
-        <v>10875</v>
+        <v>15950</v>
       </c>
     </row>
     <row r="20">
@@ -1007,25 +1007,25 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>70</v>
+        <v>120</v>
       </c>
       <c r="C20" t="n">
         <v>130</v>
       </c>
       <c r="D20" t="n">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="E20" t="n">
         <v>110</v>
       </c>
       <c r="F20" t="n">
-        <v>630</v>
+        <v>570</v>
       </c>
       <c r="G20" t="n">
-        <v>645</v>
+        <v>465</v>
       </c>
       <c r="H20" t="n">
-        <v>5400</v>
+        <v>7200</v>
       </c>
       <c r="I20" t="n">
         <v>15950</v>
@@ -1042,22 +1042,22 @@
         <v>130</v>
       </c>
       <c r="D21" t="n">
-        <v>150</v>
+        <v>60</v>
       </c>
       <c r="E21" t="n">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="F21" t="n">
-        <v>650</v>
+        <v>730</v>
       </c>
       <c r="G21" t="n">
-        <v>255</v>
+        <v>455</v>
       </c>
       <c r="H21" t="n">
-        <v>6000</v>
+        <v>5400</v>
       </c>
       <c r="I21" t="n">
-        <v>13050</v>
+        <v>15950</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
montando gráficos e tabela com valores finais
</commit_message>
<xml_diff>
--- a/P4/simulacao.xlsx
+++ b/P4/simulacao.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Simulação" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,12 +471,22 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>lucro A</t>
+          <t>receita A</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>lucro B</t>
+          <t>receita B</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Receita Total</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Dias com produção menor que demanda</t>
         </is>
       </c>
     </row>
@@ -485,28 +495,37 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>130</v>
+        <v>90</v>
       </c>
       <c r="C2" t="n">
         <v>130</v>
       </c>
       <c r="D2" t="n">
-        <v>80</v>
+        <v>200</v>
       </c>
       <c r="E2" t="n">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="F2" t="n">
-        <v>743</v>
+        <v>552</v>
       </c>
       <c r="G2" t="n">
-        <v>560</v>
+        <v>401</v>
       </c>
       <c r="H2" t="n">
-        <v>7200</v>
+        <v>1500</v>
       </c>
       <c r="I2" t="n">
-        <v>10875</v>
+        <v>8700</v>
+      </c>
+      <c r="M2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" t="n">
+        <v>309300</v>
+      </c>
+      <c r="O2" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="3">
@@ -517,25 +536,25 @@
         <v>80</v>
       </c>
       <c r="C3" t="n">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="D3" t="n">
-        <v>75</v>
+        <v>150</v>
       </c>
       <c r="E3" t="n">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="F3" t="n">
-        <v>443</v>
+        <v>572</v>
       </c>
       <c r="G3" t="n">
-        <v>255</v>
+        <v>421</v>
       </c>
       <c r="H3" t="n">
-        <v>6750</v>
+        <v>3000</v>
       </c>
       <c r="I3" t="n">
-        <v>10875</v>
+        <v>13050</v>
       </c>
     </row>
     <row r="4">
@@ -543,28 +562,28 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="C4" t="n">
-        <v>130</v>
+        <v>95</v>
       </c>
       <c r="D4" t="n">
+        <v>75</v>
+      </c>
+      <c r="E4" t="n">
         <v>60</v>
       </c>
-      <c r="E4" t="n">
-        <v>110</v>
-      </c>
       <c r="F4" t="n">
-        <v>603</v>
+        <v>302</v>
       </c>
       <c r="G4" t="n">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="H4" t="n">
-        <v>5400</v>
+        <v>6750</v>
       </c>
       <c r="I4" t="n">
-        <v>15950</v>
+        <v>8700</v>
       </c>
     </row>
     <row r="5">
@@ -584,10 +603,10 @@
         <v>110</v>
       </c>
       <c r="F5" t="n">
-        <v>723</v>
+        <v>500</v>
       </c>
       <c r="G5" t="n">
-        <v>410</v>
+        <v>546</v>
       </c>
       <c r="H5" t="n">
         <v>7200</v>
@@ -604,25 +623,25 @@
         <v>100</v>
       </c>
       <c r="C6" t="n">
-        <v>160</v>
+        <v>130</v>
       </c>
       <c r="D6" t="n">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="E6" t="n">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="F6" t="n">
-        <v>343</v>
+        <v>630</v>
       </c>
       <c r="G6" t="n">
-        <v>400</v>
+        <v>536</v>
       </c>
       <c r="H6" t="n">
-        <v>5400</v>
+        <v>6750</v>
       </c>
       <c r="I6" t="n">
-        <v>18850</v>
+        <v>15950</v>
       </c>
     </row>
     <row r="7">
@@ -633,25 +652,25 @@
         <v>130</v>
       </c>
       <c r="C7" t="n">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="D7" t="n">
-        <v>150</v>
+        <v>80</v>
       </c>
       <c r="E7" t="n">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="F7" t="n">
-        <v>500</v>
+        <v>320</v>
       </c>
       <c r="G7" t="n">
-        <v>400</v>
+        <v>531</v>
       </c>
       <c r="H7" t="n">
-        <v>10500</v>
+        <v>7200</v>
       </c>
       <c r="I7" t="n">
-        <v>13050</v>
+        <v>10875</v>
       </c>
     </row>
     <row r="8">
@@ -659,13 +678,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="C8" t="n">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="D8" t="n">
-        <v>150</v>
+        <v>60</v>
       </c>
       <c r="E8" t="n">
         <v>110</v>
@@ -674,10 +693,10 @@
         <v>500</v>
       </c>
       <c r="G8" t="n">
-        <v>400</v>
+        <v>626</v>
       </c>
       <c r="H8" t="n">
-        <v>3000</v>
+        <v>5400</v>
       </c>
       <c r="I8" t="n">
         <v>15950</v>
@@ -691,7 +710,7 @@
         <v>90</v>
       </c>
       <c r="C9" t="n">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="D9" t="n">
         <v>150</v>
@@ -703,13 +722,13 @@
         <v>500</v>
       </c>
       <c r="G9" t="n">
-        <v>400</v>
+        <v>636</v>
       </c>
       <c r="H9" t="n">
         <v>4500</v>
       </c>
       <c r="I9" t="n">
-        <v>7550</v>
+        <v>11750</v>
       </c>
     </row>
     <row r="10">
@@ -717,28 +736,28 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="C10" t="n">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="D10" t="n">
         <v>180</v>
       </c>
       <c r="E10" t="n">
-        <v>75</v>
+        <v>110</v>
       </c>
       <c r="F10" t="n">
         <v>500</v>
       </c>
       <c r="G10" t="n">
-        <v>400</v>
+        <v>556</v>
       </c>
       <c r="H10" t="n">
-        <v>-300</v>
+        <v>2700</v>
       </c>
       <c r="I10" t="n">
-        <v>10875</v>
+        <v>15950</v>
       </c>
     </row>
     <row r="11">
@@ -749,25 +768,25 @@
         <v>100</v>
       </c>
       <c r="C11" t="n">
-        <v>95</v>
+        <v>130</v>
       </c>
       <c r="D11" t="n">
         <v>75</v>
       </c>
       <c r="E11" t="n">
-        <v>170</v>
+        <v>60</v>
       </c>
       <c r="F11" t="n">
-        <v>510</v>
+        <v>730</v>
       </c>
       <c r="G11" t="n">
-        <v>400</v>
+        <v>446</v>
       </c>
       <c r="H11" t="n">
         <v>6750</v>
       </c>
       <c r="I11" t="n">
-        <v>3650</v>
+        <v>8700</v>
       </c>
     </row>
     <row r="12">
@@ -775,28 +794,28 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C12" t="n">
         <v>110</v>
       </c>
       <c r="D12" t="n">
+        <v>75</v>
+      </c>
+      <c r="E12" t="n">
         <v>60</v>
       </c>
-      <c r="E12" t="n">
-        <v>130</v>
-      </c>
       <c r="F12" t="n">
-        <v>630</v>
+        <v>460</v>
       </c>
       <c r="G12" t="n">
-        <v>400</v>
+        <v>591</v>
       </c>
       <c r="H12" t="n">
-        <v>5400</v>
+        <v>6750</v>
       </c>
       <c r="I12" t="n">
-        <v>13250</v>
+        <v>8700</v>
       </c>
     </row>
     <row r="13">
@@ -804,28 +823,28 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="C13" t="n">
-        <v>160</v>
+        <v>95</v>
       </c>
       <c r="D13" t="n">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="E13" t="n">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="F13" t="n">
-        <v>610</v>
+        <v>500</v>
       </c>
       <c r="G13" t="n">
-        <v>400</v>
+        <v>336</v>
       </c>
       <c r="H13" t="n">
-        <v>6000</v>
+        <v>-1500</v>
       </c>
       <c r="I13" t="n">
-        <v>15950</v>
+        <v>13050</v>
       </c>
     </row>
     <row r="14">
@@ -836,25 +855,25 @@
         <v>90</v>
       </c>
       <c r="C14" t="n">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="D14" t="n">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="E14" t="n">
-        <v>75</v>
+        <v>170</v>
       </c>
       <c r="F14" t="n">
-        <v>600</v>
+        <v>500</v>
       </c>
       <c r="G14" t="n">
         <v>400</v>
       </c>
       <c r="H14" t="n">
-        <v>2700</v>
+        <v>1500</v>
       </c>
       <c r="I14" t="n">
-        <v>10875</v>
+        <v>-550</v>
       </c>
     </row>
     <row r="15">
@@ -865,25 +884,25 @@
         <v>80</v>
       </c>
       <c r="C15" t="n">
-        <v>95</v>
+        <v>130</v>
       </c>
       <c r="D15" t="n">
+        <v>80</v>
+      </c>
+      <c r="E15" t="n">
         <v>60</v>
       </c>
-      <c r="E15" t="n">
-        <v>75</v>
-      </c>
       <c r="F15" t="n">
-        <v>330</v>
+        <v>720</v>
       </c>
       <c r="G15" t="n">
         <v>400</v>
       </c>
       <c r="H15" t="n">
-        <v>5400</v>
+        <v>7200</v>
       </c>
       <c r="I15" t="n">
-        <v>10875</v>
+        <v>8700</v>
       </c>
     </row>
     <row r="16">
@@ -891,28 +910,28 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C16" t="n">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="D16" t="n">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="E16" t="n">
-        <v>170</v>
+        <v>60</v>
       </c>
       <c r="F16" t="n">
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="G16" t="n">
-        <v>515</v>
+        <v>540</v>
       </c>
       <c r="H16" t="n">
-        <v>-300</v>
+        <v>0</v>
       </c>
       <c r="I16" t="n">
-        <v>3650</v>
+        <v>8700</v>
       </c>
     </row>
     <row r="17">
@@ -920,10 +939,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="C17" t="n">
-        <v>160</v>
+        <v>110</v>
       </c>
       <c r="D17" t="n">
         <v>80</v>
@@ -932,10 +951,10 @@
         <v>110</v>
       </c>
       <c r="F17" t="n">
-        <v>620</v>
+        <v>320</v>
       </c>
       <c r="G17" t="n">
-        <v>400</v>
+        <v>560</v>
       </c>
       <c r="H17" t="n">
         <v>7200</v>
@@ -949,28 +968,28 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="C18" t="n">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="D18" t="n">
-        <v>75</v>
+        <v>150</v>
       </c>
       <c r="E18" t="n">
-        <v>90</v>
+        <v>170</v>
       </c>
       <c r="F18" t="n">
-        <v>790</v>
+        <v>500</v>
       </c>
       <c r="G18" t="n">
-        <v>400</v>
+        <v>550</v>
       </c>
       <c r="H18" t="n">
-        <v>6750</v>
+        <v>3000</v>
       </c>
       <c r="I18" t="n">
-        <v>13050</v>
+        <v>-550</v>
       </c>
     </row>
     <row r="19">
@@ -978,25 +997,25 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="C19" t="n">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="D19" t="n">
-        <v>60</v>
+        <v>200</v>
       </c>
       <c r="E19" t="n">
         <v>110</v>
       </c>
       <c r="F19" t="n">
-        <v>450</v>
+        <v>500</v>
       </c>
       <c r="G19" t="n">
-        <v>455</v>
+        <v>400</v>
       </c>
       <c r="H19" t="n">
-        <v>5400</v>
+        <v>0</v>
       </c>
       <c r="I19" t="n">
         <v>15950</v>
@@ -1007,7 +1026,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="C20" t="n">
         <v>130</v>
@@ -1016,19 +1035,19 @@
         <v>80</v>
       </c>
       <c r="E20" t="n">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="F20" t="n">
-        <v>570</v>
+        <v>660</v>
       </c>
       <c r="G20" t="n">
-        <v>465</v>
+        <v>400</v>
       </c>
       <c r="H20" t="n">
         <v>7200</v>
       </c>
       <c r="I20" t="n">
-        <v>15950</v>
+        <v>13050</v>
       </c>
     </row>
     <row r="21">
@@ -1039,25 +1058,25 @@
         <v>100</v>
       </c>
       <c r="C21" t="n">
-        <v>130</v>
+        <v>95</v>
       </c>
       <c r="D21" t="n">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="E21" t="n">
-        <v>110</v>
+        <v>75</v>
       </c>
       <c r="F21" t="n">
-        <v>730</v>
+        <v>360</v>
       </c>
       <c r="G21" t="n">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="H21" t="n">
-        <v>5400</v>
+        <v>6750</v>
       </c>
       <c r="I21" t="n">
-        <v>15950</v>
+        <v>10875</v>
       </c>
     </row>
   </sheetData>

</xml_diff>